<commit_message>
Updated Exponential_Distribution .xlsx and Readme.md files
</commit_message>
<xml_diff>
--- a/Formulas_and_Templates/Templates/Distribution/Exponential_Distribution/Exponential_Distribution.xlsx
+++ b/Formulas_and_Templates/Templates/Distribution/Exponential_Distribution/Exponential_Distribution.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\DADS\GitHub_Repositories\Excel\Formulas_and_Templates\Templates\Distribution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\DADS\GitHub_Repositories\Excel\Formulas_and_Templates\Templates\Distribution\Exponential_Distribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E31D86E6-2704-4191-8586-59A8DA0044C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308833F0-5409-4E99-AA62-A9A58FEB0428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12216" yWindow="0" windowWidth="10782" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -280,79 +280,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.16374615061559639</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.13406400920712788</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.10976232721880529</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>8.9865792823444313E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>7.357588823428847E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>6.0238842382440407E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>4.9319392788321287E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>4.0379303598931077E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3.3059777644317306E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>2.7067056647322542E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>2.2160631672466777E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1.8143590657882496E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1.4854715642866776E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1.2162012525043592E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>9.9574136735727896E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>8.152440795673243E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>6.6746539920652138E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>5.4647444894585125E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>4.4741543712331182E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>3.6631277777468361E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>2.9991153640955407E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>2.4554679806136873E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>2.010367148926715E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>1.6459494098040048E-3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>1.3475893998170934E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1407,7 +1407,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1437,7 +1437,8 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <f>_xlfn.EXPON.DIST(A2,1/$E$1,FALSE)</f>
+        <v>0.16374615061559639</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1445,13 +1446,15 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <f t="shared" ref="B3:B26" si="0">_xlfn.EXPON.DIST(A3,1/$E$1,FALSE)</f>
+        <v>0.13406400920712788</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="3">
-        <v>0</v>
+        <f>_xlfn.EXPON.DIST(7,1/E1,TRUE)-_xlfn.EXPON.DIST(3,1/E1,TRUE)</f>
+        <v>0.30221467215241998</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1459,7 +1462,8 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.10976232721880529</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1467,7 +1471,8 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>8.9865792823444313E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1475,7 +1480,8 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.357588823428847E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1483,7 +1489,8 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6.0238842382440407E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1491,7 +1498,8 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>4.9319392788321287E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1499,7 +1507,8 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>4.0379303598931077E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1507,7 +1516,8 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.3059777644317306E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1515,7 +1525,8 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.7067056647322542E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1523,7 +1534,8 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.2160631672466777E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1531,7 +1543,8 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.8143590657882496E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1539,7 +1552,8 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.4854715642866776E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1547,7 +1561,8 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.2162012525043592E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1555,7 +1570,8 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9.9574136735727896E-3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1563,7 +1579,8 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>8.152440795673243E-3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1571,7 +1588,8 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6.6746539920652138E-3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1579,7 +1597,8 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.4647444894585125E-3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1587,7 +1606,8 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>4.4741543712331182E-3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1595,7 +1615,8 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.6631277777468361E-3</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1603,7 +1624,8 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.9991153640955407E-3</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1611,7 +1633,8 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.4554679806136873E-3</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1619,7 +1642,8 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.010367148926715E-3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1627,7 +1651,8 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.6459494098040048E-3</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1635,7 +1660,8 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.3475893998170934E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>